<commit_message>
Final Burndown Chart for Sprint 1
</commit_message>
<xml_diff>
--- a/documentation/Sprint1BurnDown.xlsx
+++ b/documentation/Sprint1BurnDown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patrick\Documents\PoOP\COP4331\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Documents\School\Processes\COP4331\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13F40C65-8DBE-4E52-8EDC-3F030653516E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A243CD-7CFF-414A-B5AD-33A4E678C6C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="10080" xr2:uid="{5A07D084-3DEF-46F9-BA25-E8074F440D72}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19410" windowHeight="10080" xr2:uid="{5A07D084-3DEF-46F9-BA25-E8074F440D72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>#13</t>
   </si>
@@ -49,15 +49,34 @@
   <si>
     <t>Sprint 1 Github Issue</t>
   </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>#20</t>
+  </si>
+  <si>
+    <t>#18</t>
+  </si>
+  <si>
+    <t>We ended up using most of our time learning Flutter</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,10 +102,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -212,43 +237,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>3</c:v>
@@ -296,43 +321,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.7692307692307692</c:v>
+                  <c:v>4.615384615384615</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5384615384615383</c:v>
+                  <c:v>4.2307692307692308</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>3.8461538461538458</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4615384615384617</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0769230769230766</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6923076923076921</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2.3076923076923075</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.0769230769230766</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.846153846153846</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.6153846153846154</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.3846153846153846</c:v>
-                </c:pt>
                 <c:pt idx="8">
+                  <c:v>1.9230769230769229</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5384615384615383</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1.1538461538461537</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.92307692307692291</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.69230769230769207</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.46153846153846123</c:v>
+                  <c:v>0.76923076923076916</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.23076923076923084</c:v>
+                  <c:v>0.38461538461538414</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -414,7 +439,6 @@
         <c:axId val="1126438223"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="3"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1105,15 +1129,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1478280</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>158115</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>59055</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>158115</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1438,18 +1462,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B127DF5F-F1D4-46C2-A2A0-1779801E6B3C}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1496,7 +1520,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
         <v>43346</v>
       </c>
@@ -1540,130 +1564,160 @@
         <v>43359</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="O3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="O5" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O11">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <f>3 - ((C1-1)*(3/13))</f>
-        <v>2.7692307692307692</v>
+        <f>5 - ((C1-1)*(5/13))</f>
+        <v>4.615384615384615</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:O12" si="0">3 - ((D1-1)*(3/13))</f>
-        <v>2.5384615384615383</v>
+        <f t="shared" ref="D12:N12" si="0">5 - ((D1-1)*(5/13))</f>
+        <v>4.2307692307692308</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>2.3076923076923075</v>
+        <v>3.8461538461538458</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>2.0769230769230766</v>
+        <v>3.4615384615384617</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>1.846153846153846</v>
+        <v>3.0769230769230766</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>1.6153846153846154</v>
+        <v>2.6923076923076921</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>1.3846153846153846</v>
+        <v>2.3076923076923075</v>
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>1.1538461538461537</v>
+        <v>1.9230769230769229</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>0.92307692307692291</v>
+        <v>1.5384615384615383</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
-        <v>0.69230769230769207</v>
+        <v>1.1538461538461537</v>
       </c>
       <c r="M12">
         <f t="shared" si="0"/>
-        <v>0.46153846153846123</v>
+        <v>0.76923076923076916</v>
       </c>
       <c r="N12">
         <f t="shared" si="0"/>
-        <v>0.23076923076923084</v>
+        <v>0.38461538461538414</v>
       </c>
       <c r="O12">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D12:O12" si="1">3 - ((O1-1)*(3/13))</f>
         <v>0</v>
       </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I14:O14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>